<commit_message>
Changed PatientNumber from Guid to string Added option to choose Zip file for importing Added checking if patient exists before adding, if exists only manipulation is added.
</commit_message>
<xml_diff>
--- a/Clinics/Output/stats_31-08-2014.xlsx
+++ b/Clinics/Output/stats_31-08-2014.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Joined" sheetId="1" r:id="Re1c180249f3140ef"/>
+    <sheet name="Joined" sheetId="1" r:id="R1e61002c58b74a83"/>
   </sheets>
 </workbook>
 </file>
@@ -124,7 +124,7 @@
   </sheetData>
   <headerFooter/>
   <tableParts>
-    <tablePart r:id="R87233126d11f454d"/>
+    <tablePart r:id="R6e08d39b86824339"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>